<commit_message>
This message describes what was changed in the current commit
</commit_message>
<xml_diff>
--- a/docs/other_responses_file.xlsx
+++ b/docs/other_responses_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnahiReyes\gh_projects\ra_guide\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A34FD95-FBF6-40CF-8DDB-43F293125868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A823557-3645-4075-B7B4-972BA5BE4F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2355" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="168">
   <si>
     <t>surveyid</t>
   </si>
@@ -528,23 +528,26 @@
     <t>Variable</t>
   </si>
   <si>
-    <t>Proposal of label</t>
-  </si>
-  <si>
     <t>Frequency</t>
   </si>
   <si>
     <t>disadvantages_pos / disadvantages_pos_b / disadvantages_pos_c</t>
   </si>
   <si>
-    <t xml:space="preserve">Number </t>
+    <t>Number of category</t>
+  </si>
+  <si>
+    <t>Label of new category</t>
+  </si>
+  <si>
+    <t>disadvantages_pos_other_c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -586,6 +589,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD3D3D3"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -633,7 +642,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -657,20 +666,23 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="60">
+  <dxfs count="40">
     <dxf>
       <fill>
         <patternFill>
@@ -703,146 +715,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1401,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1453,127 +1325,135 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2" s="8"/>
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1605791</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J3" s="8"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="J2" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="H3" s="4">
-        <v>5</v>
-      </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>128</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="J4" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="K4" s="3"/>
+      <c r="C4" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="H4" s="8">
+        <v>9</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="A5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" s="8">
+        <v>4</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -1583,358 +1463,349 @@
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="H7" s="3">
-        <v>13</v>
-      </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="C7" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" t="s">
-        <v>131</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="H8" s="4">
-        <v>14</v>
-      </c>
-      <c r="J8" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H8" s="8">
+        <v>6</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" t="s">
-        <v>132</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="J9" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="K9" s="3"/>
+      <c r="A9" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="H9" s="8">
+        <v>54</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
         <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="H10" s="3">
-        <v>1</v>
-      </c>
-      <c r="J10" s="3"/>
+        <v>80</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="J10" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="H11" s="3">
-        <v>1</v>
-      </c>
-      <c r="J11" s="3"/>
+      <c r="D11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>71</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="H12" s="8">
-        <v>6</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
       <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+      <c r="J12" s="8" t="s">
+        <v>140</v>
+      </c>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>71</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
+      <c r="J13" s="8" t="s">
+        <v>140</v>
+      </c>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8" t="s">
-        <v>140</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="H14" s="4">
+        <v>5</v>
+      </c>
+      <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" ht="39.5">
       <c r="A15" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>128</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>71</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
-      <c r="J15" s="8" t="s">
-        <v>140</v>
-      </c>
+      <c r="J15" s="8"/>
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="1:11" ht="39.5">
+    <row r="16" spans="1:11">
       <c r="A16" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>66</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>71</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
+        <v>95</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H16" s="8">
+        <v>10</v>
+      </c>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="3" t="s">
-        <v>50</v>
+      <c r="A17" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>66</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="H17" s="8">
-        <v>10</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
-      <c r="K17" s="3"/>
+      <c r="K17" s="7"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="3" t="s">
-        <v>51</v>
+      <c r="A18" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>66</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="H18" s="8">
-        <v>10</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
-      <c r="K18" s="3"/>
+      <c r="K18" s="7"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>71</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H19" s="8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -1942,7 +1813,7 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>67</v>
@@ -1951,40 +1822,42 @@
         <v>128</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>71</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
+        <v>97</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H20" s="8">
+        <v>6</v>
+      </c>
       <c r="I20" s="8"/>
-      <c r="J20" s="8" t="s">
-        <v>140</v>
-      </c>
+      <c r="J20" s="8"/>
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="3" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>67</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>71</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -1995,289 +1868,289 @@
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="8" t="s">
+      <c r="A22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="H22" s="8">
-        <v>12</v>
-      </c>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="7"/>
+      <c r="C22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="J22" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="8" t="s">
+      <c r="A23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8" t="s">
+      <c r="C23" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s">
+        <v>130</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="J24" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="K23" s="7"/>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="8" t="s">
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="K24" s="7"/>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>133</v>
-      </c>
       <c r="D25" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F25" s="9"/>
+      <c r="F25" s="9" t="s">
+        <v>99</v>
+      </c>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="7"/>
+      <c r="J25" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="K25" s="3"/>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>71</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H26" s="8">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="7"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="7" t="s">
-        <v>58</v>
+      <c r="A27" t="s">
+        <v>158</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>28</v>
+        <v>154</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F27" s="9" t="s">
-        <v>104</v>
+      <c r="F27" s="8" t="s">
+        <v>150</v>
       </c>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8" t="s">
-        <v>140</v>
-      </c>
+      <c r="I27" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J27" s="8"/>
       <c r="K27" s="7"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="7" t="s">
-        <v>59</v>
+      <c r="A28" t="s">
+        <v>159</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>67</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>29</v>
+        <v>155</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="H28" s="8">
-        <v>54</v>
-      </c>
-      <c r="I28" s="8"/>
+        <v>71</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="10" t="s">
+        <v>116</v>
+      </c>
       <c r="J28" s="8"/>
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="7" t="s">
-        <v>60</v>
+      <c r="A29" t="s">
+        <v>160</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>106</v>
+        <v>167</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>152</v>
       </c>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
+      <c r="I29" s="10" t="s">
+        <v>116</v>
+      </c>
       <c r="J29" s="8"/>
       <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="7" t="s">
-        <v>44</v>
+      <c r="A30" t="s">
+        <v>161</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>67</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>14</v>
+        <v>157</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>107</v>
+        <v>71</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>153</v>
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
+      <c r="I30" s="10" t="s">
+        <v>116</v>
+      </c>
       <c r="J30" s="8"/>
-      <c r="K30" s="7"/>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
+      <c r="J31" s="8" t="s">
+        <v>140</v>
+      </c>
       <c r="K31" s="7"/>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="7" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
@@ -2287,54 +2160,50 @@
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>133</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H33" s="8">
-        <v>4</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
       <c r="K33" s="7"/>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="7" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="H34" s="8">
         <v>4</v>
@@ -2344,81 +2213,78 @@
       <c r="K34" s="7"/>
     </row>
     <row r="35" spans="1:11">
-      <c r="A35" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" s="8" t="s">
+      <c r="A35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="H35" s="8">
-        <v>9</v>
-      </c>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="7"/>
+      <c r="C35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H35" s="3">
+        <v>1</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>65</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="H36" s="8">
-        <v>4</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
       <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
+      <c r="J36" s="8" t="s">
+        <v>140</v>
+      </c>
       <c r="K36" s="7"/>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>66</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
@@ -2427,48 +2293,51 @@
       <c r="K37" s="7"/>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="7"/>
+      <c r="A38" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" t="s">
+        <v>133</v>
+      </c>
+      <c r="D38" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H38" s="3">
+        <v>1</v>
+      </c>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="7" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
@@ -2477,50 +2346,52 @@
       <c r="K39" s="7"/>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" t="s">
-        <v>144</v>
+      <c r="A40" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>67</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>141</v>
+        <v>14</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="10" t="s">
-        <v>116</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H40" s="8">
+        <v>4</v>
+      </c>
+      <c r="I40" s="8"/>
       <c r="J40" s="8"/>
       <c r="K40" s="7"/>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>67</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="D41" s="8">
-        <v>1605791</v>
+        <v>143</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>142</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>71</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
@@ -2531,359 +2402,288 @@
       <c r="K41" s="7"/>
     </row>
     <row r="42" spans="1:11">
-      <c r="A42" t="s">
-        <v>146</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="J42" s="8"/>
-      <c r="K42" s="7"/>
+      <c r="A42" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" t="s">
+        <v>128</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="H42" s="3">
+        <v>13</v>
+      </c>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43" t="s">
-        <v>158</v>
+      <c r="A43" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>66</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>154</v>
+        <v>27</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F43" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="10" t="s">
+      <c r="F43" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G43" s="8" t="s">
         <v>116</v>
       </c>
+      <c r="H43" s="8">
+        <v>10</v>
+      </c>
+      <c r="I43" s="8"/>
       <c r="J43" s="8"/>
       <c r="K43" s="7"/>
     </row>
     <row r="44" spans="1:11">
-      <c r="A44" t="s">
-        <v>159</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="J44" s="8"/>
+      <c r="A44" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H44" s="4">
+        <v>14</v>
+      </c>
+      <c r="J44" s="3"/>
       <c r="K44" s="7"/>
     </row>
     <row r="45" spans="1:11">
-      <c r="A45" t="s">
-        <v>160</v>
+      <c r="A45" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>156</v>
+        <v>28</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F45" s="8" t="s">
-        <v>152</v>
+      <c r="F45" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
-      <c r="I45" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="J45" s="8"/>
-      <c r="K45" s="7"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="K45" s="3"/>
     </row>
     <row r="46" spans="1:11">
-      <c r="A46" t="s">
-        <v>161</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="J46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="7"/>
     </row>
     <row r="47" spans="1:11">
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
+      <c r="K47" s="16"/>
     </row>
     <row r="48" spans="1:11">
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-    </row>
-    <row r="49" spans="2:10">
+      <c r="D48" s="16"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="16"/>
+    </row>
+    <row r="49" spans="2:11">
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="16"/>
+    </row>
+    <row r="50" spans="2:11">
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
+      <c r="I50" s="16"/>
+      <c r="J50" s="16"/>
+      <c r="K50" s="16"/>
     </row>
   </sheetData>
   <autoFilter ref="H1:H39" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="E40">
-    <cfRule type="expression" dxfId="59" priority="51">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K46">
+    <sortCondition ref="D2:D46"/>
+  </sortState>
+  <conditionalFormatting sqref="E40 D48:F48">
+    <cfRule type="expression" dxfId="39" priority="66">
       <formula>$L40=5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="52">
+    <cfRule type="expression" dxfId="38" priority="67">
       <formula>$L40=4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="53">
+    <cfRule type="expression" dxfId="37" priority="68">
       <formula>$L40=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="54">
+    <cfRule type="expression" dxfId="36" priority="69">
       <formula>$L40=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="55">
+    <cfRule type="expression" dxfId="35" priority="70">
       <formula>$L40=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="expression" dxfId="54" priority="46">
+    <cfRule type="expression" dxfId="34" priority="61">
       <formula>$L41=5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="47">
+    <cfRule type="expression" dxfId="33" priority="62">
       <formula>$L41=4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="48">
+    <cfRule type="expression" dxfId="32" priority="63">
       <formula>$L41=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="49">
+    <cfRule type="expression" dxfId="31" priority="64">
       <formula>$L41=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="50">
+    <cfRule type="expression" dxfId="30" priority="65">
       <formula>$L41=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="expression" dxfId="49" priority="41">
+    <cfRule type="expression" dxfId="29" priority="56">
       <formula>$L42=5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="42">
+    <cfRule type="expression" dxfId="28" priority="57">
       <formula>$L42=4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="43">
+    <cfRule type="expression" dxfId="27" priority="58">
       <formula>$L42=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="44">
+    <cfRule type="expression" dxfId="26" priority="59">
       <formula>$L42=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="45">
+    <cfRule type="expression" dxfId="25" priority="60">
       <formula>$L42=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E43">
-    <cfRule type="expression" dxfId="44" priority="36">
-      <formula>$L43=5</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="37">
-      <formula>$L43=4</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="38">
-      <formula>$L43=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="39">
-      <formula>$L43=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="40">
-      <formula>$L43=1</formula>
+  <conditionalFormatting sqref="E43 C43:D45 A43:A45 D46:F46">
+    <cfRule type="expression" dxfId="24" priority="46">
+      <formula>$L44=5</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="47">
+      <formula>$L44=4</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="48">
+      <formula>$L44=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="49">
+      <formula>$L44=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="50">
+      <formula>$L44=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
-    <cfRule type="expression" dxfId="39" priority="31">
+  <conditionalFormatting sqref="E44:E45">
+    <cfRule type="expression" dxfId="19" priority="41">
+      <formula>$L45=5</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="42">
+      <formula>$L45=4</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="43">
+      <formula>$L45=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="44">
+      <formula>$L45=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="45">
+      <formula>$L45=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F40:F42">
+    <cfRule type="expression" dxfId="14" priority="36">
+      <formula>$L40=5</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="37">
+      <formula>$L40=4</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="38">
+      <formula>$L40=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="39">
+      <formula>$L40=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="40">
+      <formula>$L40=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F43:F45">
+    <cfRule type="expression" dxfId="9" priority="31">
       <formula>$L44=5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="32">
+    <cfRule type="expression" dxfId="8" priority="32">
       <formula>$L44=4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="33">
+    <cfRule type="expression" dxfId="7" priority="33">
       <formula>$L44=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="34">
+    <cfRule type="expression" dxfId="6" priority="34">
       <formula>$L44=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="35">
+    <cfRule type="expression" dxfId="5" priority="35">
       <formula>$L44=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45:E46">
-    <cfRule type="expression" dxfId="34" priority="26">
-      <formula>$L45=5</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="27">
-      <formula>$L45=4</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="28">
-      <formula>$L45=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="31" priority="29">
-      <formula>$L45=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="30">
-      <formula>$L45=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F40:F43">
-    <cfRule type="expression" dxfId="29" priority="21">
-      <formula>$L40=5</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="22">
-      <formula>$L40=4</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="23">
-      <formula>$L40=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="24">
-      <formula>$L40=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="25">
-      <formula>$L40=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F44:F46">
-    <cfRule type="expression" dxfId="24" priority="16">
-      <formula>$L44=5</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="23" priority="17">
-      <formula>$L44=4</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="18">
-      <formula>$L44=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="19">
-      <formula>$L44=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="20">
-      <formula>$L44=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D43:D46">
-    <cfRule type="expression" dxfId="19" priority="11">
-      <formula>$L43=5</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="12">
-      <formula>$L43=4</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="13">
-      <formula>$L43=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="14">
-      <formula>$L43=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="15">
-      <formula>$L43=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C43:C46">
-    <cfRule type="expression" dxfId="14" priority="6">
-      <formula>$L43=5</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="7">
-      <formula>$L43=4</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="8">
-      <formula>$L43=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="9">
-      <formula>$L43=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="10">
-      <formula>$L43=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A43:A46">
-    <cfRule type="expression" dxfId="9" priority="1">
-      <formula>$L43=5</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2">
-      <formula>$L43=4</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="3">
-      <formula>$L43=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4">
-      <formula>$L43=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5">
-      <formula>$L43=1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2896,13 +2696,13 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="19.81640625" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="2" max="2" width="19.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.26953125" customWidth="1"/>
     <col min="4" max="4" width="19.90625" customWidth="1"/>
   </cols>
@@ -2912,18 +2712,18 @@
         <v>162</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>163</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="37.5">
       <c r="A2" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>116</v>

</xml_diff>